<commit_message>
Scheme Management System implementation completed
</commit_message>
<xml_diff>
--- a/SCHEME FORMATE2.xlsx
+++ b/SCHEME FORMATE2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="49">
   <si>
     <t>Mode</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve"> UPI</t>
-  </si>
-  <si>
-    <t>_</t>
   </si>
   <si>
     <t>Card Classification</t>
@@ -190,7 +187,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,13 +214,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -358,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,12 +424,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,68 +707,68 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1183,10 +1167,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -1528,10 +1512,10 @@
         <v>23</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="19">
         <v>1.5</v>
@@ -1546,6 +1530,32 @@
         <v>12</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1.1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1578,82 +1588,82 @@
   <sheetData>
     <row r="1" ht="15.5" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -1663,112 +1673,112 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -1778,47 +1788,47 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>